<commit_message>
Definition des objectifs du projet
</commit_message>
<xml_diff>
--- a/Electronique/Carte Robot/Brochage Teensy 3.5.xlsx
+++ b/Electronique/Carte Robot/Brochage Teensy 3.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\Electronique\Carte Robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Folder\my_robot\Electronique\Carte Robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB24CB3-8E99-426D-A530-41A735B4CD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EF49CF-252F-4125-9080-E90C8BB907C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Brochage v1" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
   <si>
     <t>Labels</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>Teensy 3.5</t>
+  </si>
+  <si>
+    <t>STRAT</t>
   </si>
 </sst>
 </file>
@@ -1079,7 +1082,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,7 +1151,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="12" t="s">
+        <v>10</v>
+      </c>
       <c r="B6" s="4">
         <v>2</v>
       </c>
@@ -1189,7 +1194,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="B9" s="4">
         <v>5</v>
       </c>

</xml_diff>